<commit_message>
Updated csv for e15
</commit_message>
<xml_diff>
--- a/E15.xlsx
+++ b/E15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/ostlert_cardiff_ac_uk/Documents/Uni_Seating/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42A7DA2C-5F87-44F2-8383-53C035ABEAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9BCB54A-6C04-404A-9C48-B2B8C6832101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37215EB6-DD0B-4AA9-8297-AA089467C771}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{37215EB6-DD0B-4AA9-8297-AA089467C771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877E60B2-7E33-41C9-A283-1645A73A551C}">
   <dimension ref="A1:B191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="K181" sqref="K181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,7 +408,8 @@
         <v>1.76</v>
       </c>
       <c r="B3">
-        <v>5.4779999999999998</v>
+        <f>B2+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -416,7 +417,8 @@
         <v>1.76</v>
       </c>
       <c r="B4">
-        <v>6.3319999999999999</v>
+        <f>B3+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -424,7 +426,8 @@
         <v>1.76</v>
       </c>
       <c r="B5">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B5:B10" si="0">B4+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -432,7 +435,8 @@
         <v>1.76</v>
       </c>
       <c r="B6">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="0"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,7 +444,8 @@
         <v>1.76</v>
       </c>
       <c r="B7">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="0"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +453,8 @@
         <v>1.76</v>
       </c>
       <c r="B8">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="0"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +462,8 @@
         <v>1.76</v>
       </c>
       <c r="B9">
-        <v>10.528</v>
+        <f t="shared" si="0"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +471,8 @@
         <v>1.76</v>
       </c>
       <c r="B10">
-        <v>11.353</v>
+        <f t="shared" si="0"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,7 +496,8 @@
         <v>2.36</v>
       </c>
       <c r="B13">
-        <v>5.4779999999999998</v>
+        <f>B12+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -496,7 +505,8 @@
         <v>2.36</v>
       </c>
       <c r="B14">
-        <v>6.3319999999999999</v>
+        <f>B13+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,7 +514,8 @@
         <v>2.36</v>
       </c>
       <c r="B15">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B15:B20" si="1">B14+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -512,7 +523,8 @@
         <v>2.36</v>
       </c>
       <c r="B16">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="1"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +532,8 @@
         <v>2.36</v>
       </c>
       <c r="B17">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="1"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +541,8 @@
         <v>2.36</v>
       </c>
       <c r="B18">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="1"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +550,8 @@
         <v>2.36</v>
       </c>
       <c r="B19">
-        <v>10.528</v>
+        <f t="shared" si="1"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,7 +559,8 @@
         <v>2.36</v>
       </c>
       <c r="B20">
-        <v>11.353</v>
+        <f t="shared" si="1"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,7 +584,8 @@
         <v>2.907</v>
       </c>
       <c r="B23">
-        <v>5.4779999999999998</v>
+        <f>B22+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -576,7 +593,8 @@
         <v>2.907</v>
       </c>
       <c r="B24">
-        <v>6.3319999999999999</v>
+        <f>B23+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,7 +602,8 @@
         <v>2.907</v>
       </c>
       <c r="B25">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B25:B30" si="2">B24+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -592,7 +611,8 @@
         <v>2.907</v>
       </c>
       <c r="B26">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="2"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,7 +620,8 @@
         <v>2.907</v>
       </c>
       <c r="B27">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="2"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -608,7 +629,8 @@
         <v>2.907</v>
       </c>
       <c r="B28">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="2"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -616,7 +638,8 @@
         <v>2.907</v>
       </c>
       <c r="B29">
-        <v>10.528</v>
+        <f t="shared" si="2"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -624,7 +647,8 @@
         <v>2.907</v>
       </c>
       <c r="B30">
-        <v>11.353</v>
+        <f t="shared" si="2"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -648,7 +672,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B33">
-        <v>5.4779999999999998</v>
+        <f>B32+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -656,7 +681,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B34">
-        <v>6.3319999999999999</v>
+        <f>B33+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +690,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B35">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B35:B40" si="3">B34+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,7 +699,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B36">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="3"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,7 +708,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B37">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="3"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -688,7 +717,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B38">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="3"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +726,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B39">
-        <v>10.528</v>
+        <f t="shared" si="3"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -704,7 +735,8 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="B40">
-        <v>11.353</v>
+        <f t="shared" si="3"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -728,7 +760,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B43">
-        <v>5.4779999999999998</v>
+        <f>B42+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -736,7 +769,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B44">
-        <v>6.3319999999999999</v>
+        <f>B43+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +778,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B45">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B45:B50" si="4">B44+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -752,7 +787,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B46">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="4"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -760,7 +796,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B47">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="4"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +805,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B48">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="4"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +814,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B49">
-        <v>10.528</v>
+        <f t="shared" si="4"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +823,8 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B50">
-        <v>11.353</v>
+        <f t="shared" si="4"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +848,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B53">
-        <v>5.4779999999999998</v>
+        <f>B52+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +857,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B54">
-        <v>6.3319999999999999</v>
+        <f>B53+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -824,7 +866,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B55">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B55:B60" si="5">B54+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,7 +875,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B56">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="5"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +884,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B57">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="5"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +893,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B58">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="5"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -856,7 +902,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B59">
-        <v>10.528</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +911,8 @@
         <v>4.5789999999999997</v>
       </c>
       <c r="B60">
-        <v>11.353</v>
+        <f t="shared" si="5"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +928,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B62">
-        <v>5.4779999999999998</v>
+        <f>B61+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -888,7 +937,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B63">
-        <v>6.3319999999999999</v>
+        <f>B62+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,7 +946,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B64">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B64:B69" si="6">B63+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,7 +955,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B65">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="6"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -912,7 +964,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B66">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="6"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -920,7 +973,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B67">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="6"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -928,7 +982,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B68">
-        <v>10.528</v>
+        <f t="shared" si="6"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,7 +991,8 @@
         <v>6.2850000000000001</v>
       </c>
       <c r="B69">
-        <v>11.353</v>
+        <f t="shared" si="6"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +1008,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B71">
-        <v>5.4779999999999998</v>
+        <f>B70+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -960,7 +1017,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B72">
-        <v>6.3319999999999999</v>
+        <f>B71+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -968,7 +1026,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B73">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B73:B78" si="7">B72+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -976,7 +1035,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B74">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="7"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -984,7 +1044,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B75">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="7"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,7 +1053,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B76">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="7"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1000,7 +1062,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B77">
-        <v>10.528</v>
+        <f t="shared" si="7"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1008,7 +1071,8 @@
         <v>6.8860000000000001</v>
       </c>
       <c r="B78">
-        <v>11.353</v>
+        <f t="shared" si="7"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1024,7 +1088,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B80">
-        <v>5.4779999999999998</v>
+        <f>B79+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,7 +1097,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B81">
-        <v>6.3319999999999999</v>
+        <f>B80+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1040,7 +1106,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B82">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B82:B87" si="8">B81+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,7 +1115,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B83">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="8"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1056,7 +1124,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B84">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="8"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,7 +1133,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B85">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="8"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1072,7 +1142,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B86">
-        <v>10.528</v>
+        <f t="shared" si="8"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1080,7 +1151,8 @@
         <v>7.4420000000000002</v>
       </c>
       <c r="B87">
-        <v>11.353</v>
+        <f t="shared" si="8"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1096,7 +1168,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B89">
-        <v>5.4779999999999998</v>
+        <f>B88+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1104,7 +1177,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B90">
-        <v>6.3319999999999999</v>
+        <f>B89+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1112,7 +1186,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B91">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B91:B96" si="9">B90+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1120,7 +1195,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B92">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="9"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1128,7 +1204,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B93">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="9"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1136,7 +1213,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B94">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="9"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1144,7 +1222,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B95">
-        <v>10.528</v>
+        <f t="shared" si="9"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,7 +1231,8 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="B96">
-        <v>11.353</v>
+        <f t="shared" si="9"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,7 +1248,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B98">
-        <v>5.4779999999999998</v>
+        <f>B97+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1176,7 +1257,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B99">
-        <v>6.3319999999999999</v>
+        <f>B98+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1184,7 +1266,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B100">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B100:B105" si="10">B99+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,7 +1275,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B101">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="10"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1200,7 +1284,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B102">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="10"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1208,7 +1293,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B103">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="10"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,7 +1302,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B104">
-        <v>10.528</v>
+        <f t="shared" si="10"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1224,7 +1311,8 @@
         <v>8.5540000000000003</v>
       </c>
       <c r="B105">
-        <v>11.353</v>
+        <f t="shared" si="10"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1248,7 +1336,8 @@
         <v>10.209</v>
       </c>
       <c r="B108">
-        <v>5.4779999999999998</v>
+        <f>B107+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1256,7 +1345,8 @@
         <v>10.209</v>
       </c>
       <c r="B109">
-        <v>6.3319999999999999</v>
+        <f>B108+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1354,8 @@
         <v>10.209</v>
       </c>
       <c r="B110">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B110:B115" si="11">B109+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1363,8 @@
         <v>10.209</v>
       </c>
       <c r="B111">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="11"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,7 +1372,8 @@
         <v>10.209</v>
       </c>
       <c r="B112">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="11"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1381,8 @@
         <v>10.209</v>
       </c>
       <c r="B113">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="11"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,7 +1390,8 @@
         <v>10.209</v>
       </c>
       <c r="B114">
-        <v>10.528</v>
+        <f t="shared" si="11"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1304,7 +1399,8 @@
         <v>10.209</v>
       </c>
       <c r="B115">
-        <v>11.353</v>
+        <f t="shared" si="11"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -1328,7 +1424,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B118">
-        <v>5.4779999999999998</v>
+        <f>B117+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1433,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B119">
-        <v>6.3319999999999999</v>
+        <f>B118+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,7 +1442,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B120">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B120:B125" si="12">B119+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1451,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B121">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="12"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1460,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B122">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="12"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1469,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B123">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="12"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1478,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B124">
-        <v>10.528</v>
+        <f t="shared" si="12"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1487,8 @@
         <v>10.808999999999999</v>
       </c>
       <c r="B125">
-        <v>11.353</v>
+        <f t="shared" si="12"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1512,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B128">
-        <v>5.4779999999999998</v>
+        <f>B127+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1521,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B129">
-        <v>6.3319999999999999</v>
+        <f>B128+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -1424,7 +1530,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B130">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B130:B135" si="13">B129+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -1432,7 +1539,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B131">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="13"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1548,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B132">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="13"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1557,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B133">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="13"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1566,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B134">
-        <v>10.528</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1575,8 @@
         <v>11.364000000000001</v>
       </c>
       <c r="B135">
-        <v>11.353</v>
+        <f t="shared" si="13"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -1488,7 +1600,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B138">
-        <v>5.4779999999999998</v>
+        <f>B137+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,7 +1609,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B139">
-        <v>6.3319999999999999</v>
+        <f>B138+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1618,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B140">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B140:B145" si="14">B139+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1627,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B141">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="14"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1636,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B142">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="14"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1645,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B143">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="14"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1654,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B144">
-        <v>10.528</v>
+        <f t="shared" si="14"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -1544,7 +1663,8 @@
         <v>11.920999999999999</v>
       </c>
       <c r="B145">
-        <v>11.353</v>
+        <f t="shared" si="14"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1688,8 @@
         <v>12.47</v>
       </c>
       <c r="B148">
-        <v>5.4779999999999998</v>
+        <f>B147+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1697,8 @@
         <v>12.47</v>
       </c>
       <c r="B149">
-        <v>6.3319999999999999</v>
+        <f>B148+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1706,8 @@
         <v>12.47</v>
       </c>
       <c r="B150">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B150:B155" si="15">B149+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1715,8 @@
         <v>12.47</v>
       </c>
       <c r="B151">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="15"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,7 +1724,8 @@
         <v>12.47</v>
       </c>
       <c r="B152">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="15"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,7 +1733,8 @@
         <v>12.47</v>
       </c>
       <c r="B153">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="15"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -1616,7 +1742,8 @@
         <v>12.47</v>
       </c>
       <c r="B154">
-        <v>10.528</v>
+        <f t="shared" si="15"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1751,8 @@
         <v>12.47</v>
       </c>
       <c r="B155">
-        <v>11.353</v>
+        <f t="shared" si="15"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -1648,7 +1776,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B158">
-        <v>5.4779999999999998</v>
+        <f>B157+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -1656,7 +1785,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B159">
-        <v>6.3319999999999999</v>
+        <f>B158+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -1664,7 +1794,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B160">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B160:B165" si="16">B159+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,7 +1803,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B161">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="16"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -1680,7 +1812,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B162">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="16"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -1688,7 +1821,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B163">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="16"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,7 +1830,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B164">
-        <v>10.528</v>
+        <f t="shared" si="16"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,7 +1839,8 @@
         <v>13.021000000000001</v>
       </c>
       <c r="B165">
-        <v>11.353</v>
+        <f t="shared" si="16"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,7 +1864,8 @@
         <v>13.573</v>
       </c>
       <c r="B168">
-        <v>5.4779999999999998</v>
+        <f>B167+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -1736,7 +1873,8 @@
         <v>13.573</v>
       </c>
       <c r="B169">
-        <v>6.3319999999999999</v>
+        <f>B168+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -1744,7 +1882,8 @@
         <v>13.573</v>
       </c>
       <c r="B170">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B170:B175" si="17">B169+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +1891,8 @@
         <v>13.573</v>
       </c>
       <c r="B171">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="17"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -1760,7 +1900,8 @@
         <v>13.573</v>
       </c>
       <c r="B172">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="17"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,7 +1909,8 @@
         <v>13.573</v>
       </c>
       <c r="B173">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="17"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +1918,8 @@
         <v>13.573</v>
       </c>
       <c r="B174">
-        <v>10.528</v>
+        <f t="shared" si="17"/>
+        <v>9.7099999999999973</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -1784,7 +1927,8 @@
         <v>13.573</v>
       </c>
       <c r="B175">
-        <v>11.353</v>
+        <f t="shared" si="17"/>
+        <v>10.559999999999997</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -1808,7 +1952,8 @@
         <v>14.122</v>
       </c>
       <c r="B178">
-        <v>5.4779999999999998</v>
+        <f>B177+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -1816,7 +1961,8 @@
         <v>14.122</v>
       </c>
       <c r="B179">
-        <v>6.3319999999999999</v>
+        <f>B178+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -1824,7 +1970,8 @@
         <v>14.122</v>
       </c>
       <c r="B180">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B180:B183" si="18">B179+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -1832,7 +1979,8 @@
         <v>14.122</v>
       </c>
       <c r="B181">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="18"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +1988,8 @@
         <v>14.122</v>
       </c>
       <c r="B182">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="18"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,7 +1997,8 @@
         <v>14.122</v>
       </c>
       <c r="B183">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="18"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -1872,7 +2022,8 @@
         <v>14.673</v>
       </c>
       <c r="B186">
-        <v>5.4779999999999998</v>
+        <f>B185+0.85</f>
+        <v>4.6099999999999994</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -1880,7 +2031,8 @@
         <v>14.673</v>
       </c>
       <c r="B187">
-        <v>6.3319999999999999</v>
+        <f>B186+0.85</f>
+        <v>5.4599999999999991</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -1888,7 +2040,8 @@
         <v>14.673</v>
       </c>
       <c r="B188">
-        <v>7.2069999999999999</v>
+        <f t="shared" ref="B188:B191" si="19">B187+0.85</f>
+        <v>6.3099999999999987</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -1896,7 +2049,8 @@
         <v>14.673</v>
       </c>
       <c r="B189">
-        <v>8.0489999999999995</v>
+        <f t="shared" si="19"/>
+        <v>7.1599999999999984</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -1904,7 +2058,8 @@
         <v>14.673</v>
       </c>
       <c r="B190">
-        <v>8.8759999999999994</v>
+        <f t="shared" si="19"/>
+        <v>8.009999999999998</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,7 +2067,8 @@
         <v>14.673</v>
       </c>
       <c r="B191">
-        <v>9.7010000000000005</v>
+        <f t="shared" si="19"/>
+        <v>8.8599999999999977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>